<commit_message>
fix login and register page
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -426,9 +426,86 @@
         <v>abc</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>thanh</v>
+      </c>
+      <c r="B4" t="str">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>hello</v>
+      </c>
+      <c r="B5" t="str">
+        <v>12345</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>thanh2</v>
+      </c>
+      <c r="B6" t="str">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>thanh3</v>
+      </c>
+      <c r="B7" t="str">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>thanh6</v>
+      </c>
+      <c r="B8" t="str">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>thanh7</v>
+      </c>
+      <c r="B9" t="str">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>hello1</v>
+      </c>
+      <c r="B10" t="str">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>hello23</v>
+      </c>
+      <c r="B11" t="str">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="str">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>thanh1</v>
+      </c>
+      <c r="B13" t="str">
+        <v>1234</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B13"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>